<commit_message>
Update CO & GP Examples
</commit_message>
<xml_diff>
--- a/CO_Example.xlsx
+++ b/CO_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hunter.rollinger\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC7B7AF-25E5-4AD8-A118-331E1A351778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A2BE45-E9D0-4506-B4BD-FCAFF0EC9CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16680" windowWidth="29040" windowHeight="17640" xr2:uid="{690D76FC-F046-4907-A774-8CCDFA03CFFF}"/>
+    <workbookView xWindow="1710" yWindow="780" windowWidth="20910" windowHeight="11835" xr2:uid="{690D76FC-F046-4907-A774-8CCDFA03CFFF}"/>
   </bookViews>
   <sheets>
     <sheet name="000_to_000" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
   <si>
     <t>Procedure Type</t>
   </si>
@@ -56,10 +56,6 @@
 Number</t>
   </si>
   <si>
-    <t>Unskippable
-Step</t>
-  </si>
-  <si>
     <t>Skills</t>
   </si>
   <si>
@@ -67,9 +63,6 @@
   </si>
   <si>
     <t>Dynamic Variables</t>
-  </si>
-  <si>
-    <t>Pictures</t>
   </si>
   <si>
     <t>Step Title
@@ -105,37 +98,12 @@
     <t>Overview</t>
   </si>
   <si>
-    <t>Le istruzioni che seguono per la procedura di cambio formato integrano il manuale istruzione macchina</t>
-  </si>
-  <si>
-    <t>Die folgenden Anweisungen ergänzen die Bedienungsanleitung der Maschine</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>Regole di Sicurezza</t>
-  </si>
-  <si>
     <t>Safety Rules</t>
   </si>
   <si>
-    <t>Sicherheitsvorschriften</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Prima di iniziare qualsiasi operazione, leggere attentamente le procedure di sicurezza indicate sul manuale macchina, in particolare i rischi residui
-- Indossare i dispositivi di sicurezza personali e delimitare chiaramente l’area di lavoro in cui si opera
-- Attivare il pulsante di emergenza macchina
-- Svuotare la macchina da qualsiasi restante prodotto </t>
-  </si>
-  <si>
-    <t>Die folgenden Anweisungen ergänzen die Bedienungsanleitung der Maschine: 
-- Lesen Sie, bevor Sie irgendeinen Handgriff ausführen, sorgfältig die im Maschinenhandbuch enthaltenen Sicherheitsverfahren, insbesondere die Informationen zu den Restrisiken durch
-- Tragen Sie persönliche Schutzausrüstung und grenzen Sie den Arbeitsbereich, in dem Sie arbeiten, klar ab
-- Den Not-Aus-Taster der Maschine aktivieren
-- Sämtliche in der Maschine verbliebenen Produkte entfernen</t>
-  </si>
-  <si>
     <t>Warning Before Restart</t>
   </si>
   <si>
@@ -184,31 +152,12 @@
     <t>Changeover Complete</t>
   </si>
   <si>
-    <t>Pull out E-Stop</t>
-  </si>
-  <si>
     <t>Test_2</t>
   </si>
   <si>
     <t>Test_3</t>
   </si>
   <si>
-    <t>Press Prepare to Start</t>
-  </si>
-  <si>
-    <t>Press Start to run machine</t>
-  </si>
-  <si>
-    <t>The instructions for the change over procedure supplement  the instructions in the machine manual</t>
-  </si>
-  <si>
-    <t>The instructions below supplement the machine manual: 
-- Before starting any procedure, please read carefully the safety procedure in the manual, particularly the residual risks
-- Be sure to wear all the safety devices and clearly delimit the area of the operations 
-- Activate the emergency button 
-- Empty out all residual products  from the machine</t>
-  </si>
-  <si>
     <t>R.A Jones</t>
   </si>
   <si>
@@ -239,9 +188,6 @@
     <t>Install Upper Throat Guide</t>
   </si>
   <si>
-    <t>- Press Reset button on HMI.</t>
-  </si>
-  <si>
     <t>Remove_Upper_Throat.png</t>
   </si>
   <si>
@@ -249,12 +195,6 @@
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>- Click to confirm each box to verify change parts.</t>
-  </si>
-  <si>
-    <t>- Replace cartons in magazine.</t>
   </si>
   <si>
     <t>- Wait for machine to verify RFID on changed part.
@@ -271,9 +211,6 @@
 - Step is complete once all motors read as IN POSITION.</t>
   </si>
   <si>
-    <t>- Remove any cartons currently in process.</t>
-  </si>
-  <si>
     <t>Install_Upper_Throat.png</t>
   </si>
   <si>
@@ -292,43 +229,102 @@
     <t>KEY</t>
   </si>
   <si>
-    <t>CLi100 Operator</t>
-  </si>
-  <si>
-    <t>Maintenance Technician</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>Changeover is Tool-less</t>
-  </si>
-  <si>
-    <t>- Push up (1) and pull out (2) on Upper Throat Guide to remove.</t>
-  </si>
-  <si>
-    <t>- Push in (1) and pull down (2) to install Upper Throat Guide.
+    <t>- Press and hold the Cycle Stop button on the HMI for 3 seconds to unlock the guard doors.
+- Push in (1) and pull down (2) to install Upper Throat Guide.
 - Wait for machine to verify RFID on changed part.
      - Indicator will turn GREEN when part is verified
      - Indicator will turn YELLOW when RFID is not detected
-     - Indicator will turn RED if RFID is incorrect.
+     - Indicator will turn RED if RFID is incorrect.</t>
+  </si>
+  <si>
+    <t>- Replace all change parts on the machine.
+- After replacing change parts, click the red box next to each change part to confirm replacement has been completed.</t>
+  </si>
+  <si>
+    <t>- Press and hold the Cycle Stop button on the HMI for 3 seconds to unlock the guard doors.
+- Push up (1) and pull out (2) on Upper Throat Guide to remove.</t>
+  </si>
+  <si>
+    <t>- Ensure all guard doors are closed.
 - Press Reset button on HMI.</t>
   </si>
   <si>
-    <t>MECHANICAL_MAINTENANCE_ENGINEER</t>
-  </si>
-  <si>
-    <t>ACMA_ENGINEER</t>
-  </si>
-  <si>
-    <t>ACMA_ENGINEER,MECHANICAL_MAINTENANCE_ENGINEER</t>
+    <t>- Press and hold the Cycle Stop button on the HMI for 3 seconds.
+- Replace cartons in magazine and magazine throat.</t>
+  </si>
+  <si>
+    <t>- Press and hold the Cycle Stop button on the HMI for 3 seconds to unlock the guard doors.
+- Remove all cartons from carton magazine and magazine throat.</t>
+  </si>
+  <si>
+    <t>Ensure all guard doors are closed.</t>
+  </si>
+  <si>
+    <t>Press the Reset button on the HMI.</t>
+  </si>
+  <si>
+    <t>The machine may now be started when desired using the Start button.</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>SC0_1</t>
+  </si>
+  <si>
+    <t>SC0_2</t>
+  </si>
+  <si>
+    <t>SC0_3</t>
+  </si>
+  <si>
+    <t>•  Cli100 Operator
+•  Maintenance Technician</t>
+  </si>
+  <si>
+    <t>TC0_1</t>
+  </si>
+  <si>
+    <t>TC0_2</t>
+  </si>
+  <si>
+    <t>TC0_3</t>
+  </si>
+  <si>
+    <t>•  Changeover is Tool-less</t>
+  </si>
+  <si>
+    <t>Step 
+Unskippable</t>
+  </si>
+  <si>
+    <t>Picture Name</t>
+  </si>
+  <si>
+    <t>Changeover Walkthrough</t>
+  </si>
+  <si>
+    <t>The instructions below supplement the machine manual: 
+- Before starting any procedure, please read carefully the safety procedure in the manual, particularly the residual risks.
+- Be sure to wear all the safety devices and clearly delimit the area of the operations.
+- Empty out all residual products  from the machine.</t>
+  </si>
+  <si>
+    <t>SC0_1,SC0_2,SC0_3</t>
+  </si>
+  <si>
+    <t>TC0_1,TC0_2,TC0_3</t>
+  </si>
+  <si>
+    <t>Guided Changeover.
+Size is shown at the top center of the screen at all times.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +361,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -380,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -388,11 +390,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -414,11 +436,29 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="43">
     <dxf>
       <fill>
         <patternFill>
@@ -435,6 +475,27 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
@@ -442,6 +503,27 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <bgColor theme="1" tint="0.24994659260841701"/>
         </patternFill>
@@ -456,13 +538,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <bgColor theme="1" tint="0.24994659260841701"/>
         </patternFill>
@@ -478,13 +553,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -492,12 +560,54 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <bgColor theme="1" tint="0.24994659260841701"/>
         </patternFill>
@@ -520,6 +630,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -575,13 +692,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <bgColor theme="1" tint="0.24994659260841701"/>
         </patternFill>
@@ -591,6 +701,34 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -933,10 +1071,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6656757E-CA6C-47CE-9AEA-4F080DCABDED}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,17 +1082,20 @@
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
     <col min="12" max="12" width="36.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" customWidth="1"/>
-    <col min="14" max="14" width="34.7109375" customWidth="1"/>
-    <col min="15" max="15" width="49.140625" customWidth="1"/>
-    <col min="16" max="16" width="59" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="102.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,207 +1108,197 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="N2" s="3"/>
       <c r="O2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="140.25" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
       <c r="O3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="P6" s="3"/>
     </row>
@@ -1177,26 +1308,26 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="J7" s="10"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P7" s="3"/>
     </row>
@@ -1206,28 +1337,28 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P8" s="3"/>
     </row>
@@ -1237,26 +1368,26 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="J9" s="8"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="P9" s="3"/>
     </row>
@@ -1266,26 +1397,26 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="J10" s="8"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="P10" s="3"/>
     </row>
@@ -1295,57 +1426,57 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="J11" s="8"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="102" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="P12" s="3"/>
     </row>
@@ -1355,47 +1486,59 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="J14" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="P14" s="3"/>
     </row>
@@ -1405,16 +1548,18 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="P15" s="3"/>
     </row>
@@ -1424,16 +1569,18 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="P16" s="3"/>
     </row>
@@ -1443,32 +1590,40 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F17" s="4"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F18" s="4"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="O18" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1476,21 +1631,21 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1505,139 +1660,210 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:D19">
-    <cfRule type="expression" dxfId="28" priority="47">
+  <conditionalFormatting sqref="A1:D20">
+    <cfRule type="expression" dxfId="42" priority="74">
       <formula>AND(OR(EXACT($E1,"Overview"),EXACT($E1,"overview"),EXACT($E1,"OVERVIEW")),EXACT(A1,""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D19">
-    <cfRule type="expression" dxfId="27" priority="49">
+  <conditionalFormatting sqref="A2:D20">
+    <cfRule type="expression" dxfId="41" priority="76">
       <formula>AND(AND(NOT(EXACT($E2,"Overview")),NOT(EXACT($E2,"overview")),NOT(EXACT($E2,"OVERVIEW"))),NOT(EXACT($E2,"")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:Q20">
-    <cfRule type="expression" dxfId="26" priority="24">
-      <formula>AND(OR(EXACT($E19,"Overview"),EXACT($E19,"overview"),EXACT($E19,"OVERVIEW")),EXACT(E19,""))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="25">
-      <formula>AND(AND(NOT(EXACT($E19,"Overview")),NOT(EXACT($E19,"overview")),NOT(EXACT($E19,"OVERVIEW"))),NOT(EXACT($E19,"")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:I2 K1:M3 I3 F3:F18">
-    <cfRule type="expression" dxfId="24" priority="50">
-      <formula>OR(EXACT($E1,"Overview"),EXACT($E1,"overview"),EXACT($E1,"OVERVIEW"))</formula>
+  <conditionalFormatting sqref="E2:E19">
+    <cfRule type="expression" dxfId="40" priority="20">
+      <formula>AND(SUMPRODUCT(--($A2:$P2 &lt;&gt; "")),EXACT(E2,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:Q21">
+    <cfRule type="expression" dxfId="39" priority="52">
+      <formula>AND(AND(NOT(EXACT($E20,"Overview")),NOT(EXACT($E20,"overview")),NOT(EXACT($E20,"OVERVIEW"))),NOT(EXACT($E20,"")))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="51">
+      <formula>AND(OR(EXACT($E20,"Overview"),EXACT($E20,"overview"),EXACT($E20,"OVERVIEW")),EXACT(E20,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:F19">
+    <cfRule type="expression" dxfId="37" priority="77">
+      <formula>OR(EXACT($E15,"Overview"),EXACT($E15,"overview"),EXACT($E15,"OVERVIEW"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="70">
+      <formula>OR(SEARCH("Test",$E15),SEARCH("test",$E15),SEARCH("TEST",$E15))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="71">
+      <formula>OR(SEARCH("Warning",$E15),SEARCH("warning",$E15),SEARCH("WARNING",$E15))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:I2 K2 M2 K3:L3 I3 F3:F14">
+    <cfRule type="expression" dxfId="34" priority="21">
+      <formula>OR(EXACT($H2,"Overview"),EXACT($H2,"overview"),EXACT($H2,"OVERVIEW"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:J1">
+    <cfRule type="expression" dxfId="33" priority="11">
+      <formula>OR(EXACT($H1,"Overview"),EXACT($H1,"overview"),EXACT($H1,"OVERVIEW"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:K2 M2 I3:L3 F3:F14">
+    <cfRule type="expression" dxfId="32" priority="23">
+      <formula>OR(SEARCH("Warning",$H2),SEARCH("warning",$H2),SEARCH("WARNING",$H2))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="22">
+      <formula>OR(SEARCH("Test",$H2),SEARCH("test",$H2),SEARCH("TEST",$H2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:H18">
+    <cfRule type="expression" dxfId="30" priority="2">
+      <formula>OR(SEARCH("Warning",$E3),SEARCH("warning",$E3),SEARCH("WARNING",$E3))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="3">
+      <formula>OR(EXACT($E3,"Overview"),EXACT($E3,"overview"),EXACT($E3,"OVERVIEW"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="1">
+      <formula>OR(SEARCH("Test",$E3),SEARCH("test",$E3),SEARCH("TEST",$E3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:M14">
+    <cfRule type="expression" dxfId="27" priority="25">
+      <formula>OR(SEARCH("Warning",$H4),SEARCH("warning",$H4),SEARCH("WARNING",$H4))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="26">
+      <formula>OR(EXACT($H4,"Overview"),EXACT($H4,"overview"),EXACT($H4,"OVERVIEW"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="27">
+      <formula>AND(SUMPRODUCT(--($A4:$P4 &lt;&gt; "")),EXACT(J4,""))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="24">
+      <formula>OR(SEARCH("Test",$H4),SEARCH("test",$H4),SEARCH("TEST",$H4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:M19">
     <cfRule type="expression" dxfId="23" priority="45">
-      <formula>OR(EXACT($E1,"Overview"),EXACT($E1,"overview"),EXACT($E1,"OVERVIEW"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:M2 I3:M3 F3:F18">
-    <cfRule type="expression" dxfId="22" priority="43">
-      <formula>OR(SEARCH("Test",$E1),SEARCH("test",$E1),SEARCH("TEST",$E1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="44">
-      <formula>OR(SEARCH("Warning",$E1),SEARCH("warning",$E1),SEARCH("WARNING",$E1))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H13">
-    <cfRule type="expression" dxfId="20" priority="2">
+      <formula>OR(SEARCH("Test",$E15),SEARCH("test",$E15),SEARCH("TEST",$E15))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="46">
+      <formula>OR(SEARCH("Warning",$E15),SEARCH("warning",$E15),SEARCH("WARNING",$E15))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="47">
+      <formula>OR(EXACT($E15,"Overview"),EXACT($E15,"overview"),EXACT($E15,"OVERVIEW"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:N1 E1 P1">
+    <cfRule type="expression" dxfId="20" priority="12">
+      <formula>AND(SUMPRODUCT(--($A1:$S1 &lt;&gt; "")),EXACT(E1,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:N3 F2:K2 M2:N2">
+    <cfRule type="expression" dxfId="19" priority="9">
+      <formula>AND(SUMPRODUCT(--($A2:$P2 &lt;&gt; "")),EXACT(F2,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:N19">
+    <cfRule type="expression" dxfId="18" priority="48">
+      <formula>AND(SUMPRODUCT(--($A15:$P15 &lt;&gt; "")),EXACT(J15,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="expression" dxfId="17" priority="4">
+      <formula>AND(SUMPRODUCT(--($A2:$S2 &lt;&gt; "")),EXACT(L2,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3">
+    <cfRule type="expression" dxfId="16" priority="7">
+      <formula>OR(SEARCH("Warning",$E3),SEARCH("warning",$E3),SEARCH("WARNING",$E3))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="8">
+      <formula>OR(EXACT($E3,"Overview"),EXACT($E3,"overview"),EXACT($E3,"OVERVIEW"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>OR(SEARCH("Test",$E3),SEARCH("test",$E3),SEARCH("TEST",$E3))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
-      <formula>OR(SEARCH("Warning",$E3),SEARCH("warning",$E3),SEARCH("WARNING",$E3))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
-      <formula>OR(EXACT($E3,"Overview"),EXACT($E3,"overview"),EXACT($E3,"OVERVIEW"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12:J13">
-    <cfRule type="expression" dxfId="17" priority="11">
-      <formula>OR(SEARCH("Test",$H12),SEARCH("test",$H12),SEARCH("TEST",$H12))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="12">
-      <formula>OR(SEARCH("Warning",$H12),SEARCH("warning",$H12),SEARCH("WARNING",$H12))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>OR(EXACT($H12,"Overview"),EXACT($H12,"overview"),EXACT($H12,"OVERVIEW"))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>AND(SUMPRODUCT(--($A12:$P12 &lt;&gt; "")),EXACT(J12,""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:M11 K12:M13 J14:M18">
-    <cfRule type="expression" dxfId="13" priority="18">
-      <formula>OR(SEARCH("Test",$E4),SEARCH("test",$E4),SEARCH("TEST",$E4))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="19">
-      <formula>OR(SEARCH("Warning",$E4),SEARCH("warning",$E4),SEARCH("WARNING",$E4))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20">
-      <formula>OR(EXACT($E4,"Overview"),EXACT($E4,"overview"),EXACT($E4,"OVERVIEW"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:M11 K12:M13 J14:N18">
-    <cfRule type="expression" dxfId="10" priority="21">
-      <formula>AND(SUMPRODUCT(--($A4:$P4 &lt;&gt; "")),EXACT(J4,""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1:P3 N4:N13 P4:P13 E1:E18">
-    <cfRule type="expression" dxfId="9" priority="51">
-      <formula>AND(SUMPRODUCT(--($A1:$P1 &lt;&gt; "")),EXACT(E1,""))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N14 P4:P14">
+    <cfRule type="expression" dxfId="13" priority="19">
+      <formula>AND(SUMPRODUCT(--($A4:$P4 &lt;&gt; "")),EXACT(N4,""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5 P5">
-    <cfRule type="expression" dxfId="8" priority="15">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>OR(SEARCH("Test",$E5),SEARCH("test",$E5),SEARCH("TEST",$E5))</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>OR(EXACT($E5,"Overview"),EXACT($E5,"overview"),EXACT($E5,"OVERVIEW"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>OR(SEARCH("Warning",$E5),SEARCH("warning",$E5),SEARCH("WARNING",$E5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:N14 P7:P14">
+    <cfRule type="expression" dxfId="9" priority="18">
+      <formula>OR(EXACT($E7,"Overview"),EXACT($E7,"overview"),EXACT($E7,"OVERVIEW"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="17">
+      <formula>OR(SEARCH("Warning",$E7),SEARCH("warning",$E7),SEARCH("WARNING",$E7))</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="7" priority="16">
-      <formula>OR(SEARCH("Warning",$E5),SEARCH("warning",$E5),SEARCH("WARNING",$E5))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="17">
-      <formula>OR(EXACT($E5,"Overview"),EXACT($E5,"overview"),EXACT($E5,"OVERVIEW"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N7:N13 P7:P13 O18:P18">
-    <cfRule type="expression" dxfId="5" priority="35">
       <formula>OR(SEARCH("Test",$E7),SEARCH("test",$E7),SEARCH("TEST",$E7))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="36">
-      <formula>OR(SEARCH("Warning",$E7),SEARCH("warning",$E7),SEARCH("WARNING",$E7))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="37">
-      <formula>OR(EXACT($E7,"Overview"),EXACT($E7,"overview"),EXACT($E7,"OVERVIEW"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O13">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>AND(SUMPRODUCT(--($A4:$P4 &lt;&gt; "")),EXACT(O4,""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O14:P17">
-    <cfRule type="expression" dxfId="1" priority="23">
-      <formula>AND(SUMPRODUCT(--($A14:$P14 &lt;&gt; "")),EXACT(O14,""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O18:P18">
-    <cfRule type="expression" dxfId="0" priority="38">
-      <formula>AND(SUMPRODUCT(--($A18:$P18 &lt;&gt; "")),EXACT(O18,""))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O14">
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>AND(SUMPRODUCT(--($A1:$P1 &lt;&gt; "")),EXACT(O1,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15:P18">
+    <cfRule type="expression" dxfId="5" priority="50">
+      <formula>AND(SUMPRODUCT(--($A15:$P15 &lt;&gt; "")),EXACT(O15,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19:P19">
+    <cfRule type="expression" dxfId="4" priority="62">
+      <formula>OR(SEARCH("Test",$E19),SEARCH("test",$E19),SEARCH("TEST",$E19))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="63">
+      <formula>OR(SEARCH("Warning",$E19),SEARCH("warning",$E19),SEARCH("WARNING",$E19))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="64">
+      <formula>OR(EXACT($E19,"Overview"),EXACT($E19,"overview"),EXACT($E19,"OVERVIEW"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="65">
+      <formula>AND(SUMPRODUCT(--($A19:$P19 &lt;&gt; "")),EXACT(O19,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P3">
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>AND(SUMPRODUCT(--($A2:$P2 &lt;&gt; "")),EXACT(P2,""))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="1095" yWindow="389" count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Description DE" prompt="Enter the Step Description in Deutch_x000a_" sqref="P2:P4 P6" xr:uid="{21FF87D2-C46A-4131-B2E5-E2DCE3845CBC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Description EN" prompt="Enter the Step Description in English_x000a_" sqref="O2:O13" xr:uid="{9B25A306-0B89-48DD-AB17-592DF494D141}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Description IT" prompt="Enter the Step Description in Italian" sqref="N2:N4 N6" xr:uid="{00B2D700-437C-42BF-833F-C08636B48E31}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Title Deutch" prompt="Enter the Step Title in Deutch_x000a_" sqref="M2:M4 M6" xr:uid="{D4FC1BEF-92F5-4921-AEA8-8641DDC1B8C7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Title EN" prompt="Enter the Step Title in English" sqref="L2:L4 L6" xr:uid="{FBB4FC1F-D4EA-433A-AD33-56AB72C61DC4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Title IT" prompt="Enter the Step Title in Italian" sqref="K2:K4 K6" xr:uid="{F5B2BCFE-D681-49DD-B2AD-F9ABCF2FB596}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pictures" prompt="Insert step picture name with its file extension._x000a__x000a_If you want add more than one picture separate them by comma." sqref="J6 J2:J4" xr:uid="{6E699918-84CA-46B0-BAEC-1927C9235DD0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Version" prompt="Insert procedure version in the format that you like" sqref="D2:D19" xr:uid="{F3BD6E19-8C0C-4434-801D-C6775B97CADA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Author" prompt="Insert procedure Author" sqref="B2:B19" xr:uid="{DE0A594A-860F-47CD-B9BC-F88117DCBB85}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creation Date" prompt="Insert Creation Date" sqref="C2:C19" xr:uid="{273D012A-2E78-4F26-877C-BE1366B11E4E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Description DE" prompt="Enter the Step Description in Deutch_x000a_" sqref="P6 P2:P4" xr:uid="{8CACC4BB-4DEF-4B04-8D79-C276972EAEE7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Description EN" prompt="Enter the Step Description in English_x000a_" sqref="O2:O14" xr:uid="{15D47051-52E4-43F8-9924-ADB2B25282B9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Description IT" prompt="Enter the Step Description in Italian" sqref="N6 N2:N4" xr:uid="{73275755-5773-444B-A091-1D5300FEBDC9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Title Deutch" prompt="Enter the Step Title in Deutch_x000a_" sqref="M6 M2:M4" xr:uid="{2BD9B964-1EBD-457A-BC43-7E95852D0C9F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Title EN" prompt="Enter the Step Title in English" sqref="L6 L2:L4" xr:uid="{90511BFE-4B70-48E9-9E9B-2103FA8B5DAE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Step Title IT" prompt="Enter the Step Title in Italian" sqref="K2:K4 K6" xr:uid="{25B47E06-0E05-4155-9899-DDEDFBEE76C5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pictures" prompt="Insert step picture name with its file extension._x000a__x000a_If you want add more than one picture separate them by comma." sqref="J2:J4 J6 F2:I2" xr:uid="{C17F4867-025D-4AB3-879A-6CF04130C6C6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Version" prompt="Insert procedure version in the format that you like" sqref="D2:D20" xr:uid="{F3BD6E19-8C0C-4434-801D-C6775B97CADA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Author" prompt="Insert procedure Author" sqref="B2:B20" xr:uid="{DE0A594A-860F-47CD-B9BC-F88117DCBB85}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creation Date" prompt="Insert Creation Date" sqref="C2:C20" xr:uid="{273D012A-2E78-4F26-877C-BE1366B11E4E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1645,46 +1871,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D9C3E6-96F9-4FB4-87B6-863F165B5803}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1694,38 +1922,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E1CCD9-58C7-4FAD-AB69-08ED219C048F}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>